<commit_message>
박자 정보 추가. crash 방지-안정성 향상.  악보 수정 - Moon River, El Condor Pasa, etc..
</commit_message>
<xml_diff>
--- a/tools_n_data/umigamierumachi-kiki-ghibri.xlsx
+++ b/tools_n_data/umigamierumachi-kiki-ghibri.xlsx
@@ -96,7 +96,7 @@
         <family val="3"/>
         <charset val="129"/>
       </rPr>
-      <t xml:space="preserve">작성자메모</t>
+      <t xml:space="preserve">메모</t>
     </r>
   </si>
   <si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">#source</t>
   </si>
   <si>
-    <t xml:space="preserve">umigamierumachi.mp4</t>
+    <t xml:space="preserve">umigamierumachi.mp3</t>
   </si>
   <si>
     <t xml:space="preserve">#thumbnail</t>
@@ -506,7 +506,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -544,10 +544,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -675,8 +671,8 @@
   </sheetPr>
   <dimension ref="A1:CQ218"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -694,7 +690,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="96" style="0" width="3.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -748,83 +744,83 @@
       </c>
       <c r="AH2" s="6"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
       <c r="AH3" s="6"/>
     </row>
-    <row r="4" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
       <c r="AH4" s="6"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
       <c r="AH5" s="6"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="11"/>
@@ -851,86 +847,86 @@
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
       <c r="AH7" s="6"/>
     </row>
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
       <c r="AH8" s="6"/>
     </row>
     <row r="9" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
       <c r="AH9" s="6"/>
     </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,7 +934,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="7" t="n">
-        <v>0</v>
+        <v>2208</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -965,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="7" t="n">
-        <v>96</v>
+        <v>104.5</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -991,7 +987,7 @@
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="11"/>
@@ -1014,28 +1010,28 @@
       </c>
       <c r="AH12" s="6"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
+    <row r="13" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
       <c r="R13" s="5" t="s">
         <v>2</v>
       </c>
@@ -1045,7 +1041,7 @@
       <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="11"/>
@@ -1069,22 +1065,22 @@
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
       <c r="AH15" s="6"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,14 +1089,14 @@
     <row r="17" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AH17" s="6"/>
     </row>
-    <row r="18" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
+    <row r="18" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="16"/>
       <c r="J18" s="2"/>
-      <c r="R18" s="18"/>
-      <c r="Z18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="Z18" s="16"/>
       <c r="AH18" s="8" t="s">
         <v>27</v>
       </c>
@@ -1170,22 +1166,22 @@
       <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="D19" s="19"/>
-      <c r="J19" s="17" t="s">
+      <c r="B19" s="16"/>
+      <c r="D19" s="18"/>
+      <c r="J19" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="19"/>
+      <c r="L19" s="18"/>
       <c r="N19" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="X19" s="19"/>
-      <c r="Z19" s="17"/>
+      <c r="R19" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Z19" s="16"/>
       <c r="AB19" s="0" t="n">
         <v>0</v>
       </c>
@@ -1212,7 +1208,7 @@
       <c r="Q20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R20" s="17"/>
+      <c r="R20" s="16"/>
       <c r="T20" s="0" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1235,7 @@
       <c r="A21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="R21" s="17"/>
+      <c r="R21" s="16"/>
       <c r="Y21" s="0" t="n">
         <v>0</v>
       </c>
@@ -1265,38 +1261,38 @@
       <c r="A23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="20"/>
-      <c r="W23" s="20"/>
-      <c r="X23" s="20"/>
-      <c r="Y23" s="20"/>
-      <c r="Z23" s="20"/>
-      <c r="AA23" s="20"/>
-      <c r="AB23" s="20"/>
-      <c r="AC23" s="20"/>
-      <c r="AD23" s="20"/>
-      <c r="AE23" s="20"/>
-      <c r="AF23" s="20"/>
-      <c r="AG23" s="20"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AF23" s="19"/>
+      <c r="AG23" s="19"/>
       <c r="AH23" s="8" t="s">
         <v>27</v>
       </c>
@@ -1325,13 +1321,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
+    <row r="26" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="16"/>
       <c r="J26" s="2"/>
-      <c r="R26" s="17"/>
+      <c r="R26" s="16"/>
       <c r="Z26" s="2"/>
       <c r="AH26" s="8" t="s">
         <v>27</v>
@@ -1402,37 +1398,37 @@
       <c r="A27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="D27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="J27" s="17" t="s">
+      <c r="B27" s="16"/>
+      <c r="D27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="J27" s="16" t="s">
         <v>29</v>
       </c>
       <c r="N27" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="P27" s="19"/>
-      <c r="R27" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" s="19"/>
-      <c r="V27" s="19"/>
-      <c r="X27" s="19"/>
-      <c r="Z27" s="17"/>
+      <c r="P27" s="18"/>
+      <c r="R27" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Z27" s="16"/>
       <c r="AB27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="AC27" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="AD27" s="19" t="s">
+      <c r="AD27" s="18" t="s">
         <v>39</v>
       </c>
       <c r="AE27" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="AF27" s="19" t="s">
+      <c r="AF27" s="18" t="s">
         <v>41</v>
       </c>
       <c r="AH27" s="8" t="s">
@@ -1443,7 +1439,7 @@
       <c r="A28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="17" t="n">
+      <c r="B28" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -1484,7 +1480,7 @@
       <c r="A29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="17"/>
+      <c r="B29" s="16"/>
       <c r="E29" s="0" t="s">
         <v>30</v>
       </c>
@@ -1507,38 +1503,38 @@
       <c r="A31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="20"/>
-      <c r="Z31" s="20"/>
-      <c r="AA31" s="20"/>
-      <c r="AB31" s="20"/>
-      <c r="AC31" s="20"/>
-      <c r="AD31" s="20"/>
-      <c r="AE31" s="20"/>
-      <c r="AF31" s="20"/>
-      <c r="AG31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="19"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="19"/>
       <c r="AH31" s="8" t="s">
         <v>27</v>
       </c>
@@ -1567,14 +1563,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="s">
+    <row r="34" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="R34" s="17"/>
-      <c r="Z34" s="17"/>
+      <c r="R34" s="16"/>
+      <c r="Z34" s="16"/>
       <c r="AH34" s="8" t="s">
         <v>27</v>
       </c>
@@ -1644,27 +1640,27 @@
       <c r="A35" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" s="19"/>
-      <c r="J35" s="17" t="s">
+      <c r="B35" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="18"/>
+      <c r="J35" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L35" s="19"/>
+      <c r="L35" s="18"/>
       <c r="N35" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="R35" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="X35" s="19"/>
-      <c r="Z35" s="17"/>
+      <c r="R35" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" s="18"/>
+      <c r="V35" s="18"/>
+      <c r="X35" s="18"/>
+      <c r="Z35" s="16"/>
       <c r="AB35" s="0" t="n">
         <v>0</v>
       </c>
@@ -1694,7 +1690,7 @@
       <c r="Q36" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R36" s="17"/>
+      <c r="R36" s="16"/>
       <c r="T36" s="0" t="s">
         <v>29</v>
       </c>
@@ -1727,7 +1723,7 @@
       <c r="E37" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R37" s="17"/>
+      <c r="R37" s="16"/>
       <c r="Y37" s="0" t="n">
         <v>0</v>
       </c>
@@ -1753,38 +1749,38 @@
       <c r="A39" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="20"/>
-      <c r="X39" s="20"/>
-      <c r="Y39" s="20"/>
-      <c r="Z39" s="20"/>
-      <c r="AA39" s="20"/>
-      <c r="AB39" s="20"/>
-      <c r="AC39" s="20"/>
-      <c r="AD39" s="20"/>
-      <c r="AE39" s="20"/>
-      <c r="AF39" s="20"/>
-      <c r="AG39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AC39" s="19"/>
+      <c r="AD39" s="19"/>
+      <c r="AE39" s="19"/>
+      <c r="AF39" s="19"/>
+      <c r="AG39" s="19"/>
       <c r="AH39" s="8" t="s">
         <v>27</v>
       </c>
@@ -1813,14 +1809,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="16" t="s">
+    <row r="42" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B42" s="2"/>
       <c r="J42" s="2"/>
-      <c r="R42" s="17"/>
-      <c r="Z42" s="17"/>
+      <c r="R42" s="16"/>
+      <c r="Z42" s="16"/>
       <c r="AH42" s="8" t="s">
         <v>27</v>
       </c>
@@ -1890,24 +1886,24 @@
       <c r="A43" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="D43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="J43" s="17" t="s">
+      <c r="B43" s="16"/>
+      <c r="D43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="J43" s="16" t="s">
         <v>29</v>
       </c>
       <c r="N43" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="P43" s="19"/>
-      <c r="R43" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="X43" s="19"/>
-      <c r="Z43" s="17"/>
+      <c r="P43" s="18"/>
+      <c r="R43" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" s="18"/>
+      <c r="V43" s="18"/>
+      <c r="X43" s="18"/>
+      <c r="Z43" s="16"/>
       <c r="AB43" s="0" t="n">
         <v>0</v>
       </c>
@@ -1931,7 +1927,7 @@
       <c r="A44" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="17" t="n">
+      <c r="B44" s="16" t="n">
         <v>0</v>
       </c>
       <c r="F44" s="0" t="n">
@@ -1972,15 +1968,15 @@
       <c r="A45" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="17"/>
+      <c r="B45" s="16"/>
       <c r="E45" s="0" t="s">
         <v>30</v>
       </c>
       <c r="Z45" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD45" s="19"/>
-      <c r="AF45" s="19"/>
+      <c r="AD45" s="18"/>
+      <c r="AF45" s="18"/>
       <c r="AH45" s="8" t="s">
         <v>27</v>
       </c>
@@ -1997,38 +1993,38 @@
       <c r="A47" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="20"/>
-      <c r="R47" s="20"/>
-      <c r="S47" s="20"/>
-      <c r="T47" s="20"/>
-      <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
-      <c r="W47" s="20"/>
-      <c r="X47" s="20"/>
-      <c r="Y47" s="20"/>
-      <c r="Z47" s="20"/>
-      <c r="AA47" s="20"/>
-      <c r="AB47" s="20"/>
-      <c r="AC47" s="20"/>
-      <c r="AD47" s="20"/>
-      <c r="AE47" s="20"/>
-      <c r="AF47" s="20"/>
-      <c r="AG47" s="20"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="19"/>
+      <c r="AA47" s="19"/>
+      <c r="AB47" s="19"/>
+      <c r="AC47" s="19"/>
+      <c r="AD47" s="19"/>
+      <c r="AE47" s="19"/>
+      <c r="AF47" s="19"/>
+      <c r="AG47" s="19"/>
       <c r="AH47" s="8" t="s">
         <v>27</v>
       </c>
@@ -2057,14 +2053,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="16" t="s">
+    <row r="50" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="R50" s="17"/>
-      <c r="Z50" s="17"/>
+      <c r="R50" s="16"/>
+      <c r="Z50" s="16"/>
       <c r="AH50" s="8" t="s">
         <v>27</v>
       </c>
@@ -2134,19 +2130,19 @@
       <c r="A51" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" s="19" t="n">
+      <c r="B51" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="18" t="n">
         <v>0</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J51" s="16" t="s">
         <v>29</v>
       </c>
       <c r="K51" s="0" t="s">
@@ -2164,19 +2160,19 @@
       <c r="O51" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="P51" s="19" t="n">
+      <c r="P51" s="18" t="n">
         <v>0</v>
       </c>
       <c r="Q51" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="R51" s="17"/>
-      <c r="T51" s="19"/>
-      <c r="V51" s="19" t="s">
+      <c r="R51" s="16"/>
+      <c r="T51" s="18"/>
+      <c r="V51" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X51" s="19"/>
-      <c r="Z51" s="17" t="n">
+      <c r="X51" s="18"/>
+      <c r="Z51" s="16" t="n">
         <v>0</v>
       </c>
       <c r="AA51" s="0" t="n">
@@ -2205,8 +2201,8 @@
       <c r="R52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V52" s="19"/>
-      <c r="X52" s="19" t="s">
+      <c r="V52" s="18"/>
+      <c r="X52" s="18" t="s">
         <v>32</v>
       </c>
       <c r="Y52" s="0" t="s">
@@ -2238,10 +2234,10 @@
       <c r="T53" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="V53" s="19"/>
-      <c r="X53" s="19"/>
-      <c r="AD53" s="19"/>
-      <c r="AF53" s="19"/>
+      <c r="V53" s="18"/>
+      <c r="X53" s="18"/>
+      <c r="AD53" s="18"/>
+      <c r="AF53" s="18"/>
       <c r="AH53" s="8" t="s">
         <v>27</v>
       </c>
@@ -2258,38 +2254,38 @@
       <c r="A55" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
-      <c r="M55" s="20"/>
-      <c r="N55" s="20"/>
-      <c r="O55" s="20"/>
-      <c r="P55" s="20"/>
-      <c r="Q55" s="20"/>
-      <c r="R55" s="20"/>
-      <c r="S55" s="20"/>
-      <c r="T55" s="20"/>
-      <c r="U55" s="20"/>
-      <c r="V55" s="20"/>
-      <c r="W55" s="20"/>
-      <c r="X55" s="20"/>
-      <c r="Y55" s="20"/>
-      <c r="Z55" s="20"/>
-      <c r="AA55" s="20"/>
-      <c r="AB55" s="20"/>
-      <c r="AC55" s="20"/>
-      <c r="AD55" s="20"/>
-      <c r="AE55" s="20"/>
-      <c r="AF55" s="20"/>
-      <c r="AG55" s="20"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+      <c r="P55" s="19"/>
+      <c r="Q55" s="19"/>
+      <c r="R55" s="19"/>
+      <c r="S55" s="19"/>
+      <c r="T55" s="19"/>
+      <c r="U55" s="19"/>
+      <c r="V55" s="19"/>
+      <c r="W55" s="19"/>
+      <c r="X55" s="19"/>
+      <c r="Y55" s="19"/>
+      <c r="Z55" s="19"/>
+      <c r="AA55" s="19"/>
+      <c r="AB55" s="19"/>
+      <c r="AC55" s="19"/>
+      <c r="AD55" s="19"/>
+      <c r="AE55" s="19"/>
+      <c r="AF55" s="19"/>
+      <c r="AG55" s="19"/>
       <c r="AH55" s="8" t="s">
         <v>27</v>
       </c>
@@ -2318,14 +2314,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="s">
+    <row r="58" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B58" s="2"/>
       <c r="J58" s="2"/>
-      <c r="R58" s="17"/>
-      <c r="Z58" s="17"/>
+      <c r="R58" s="16"/>
+      <c r="Z58" s="16"/>
       <c r="AJ58" s="8" t="s">
         <v>27</v>
       </c>
@@ -2393,35 +2389,35 @@
       <c r="A59" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="F59" s="19"/>
+      <c r="B59" s="16"/>
+      <c r="F59" s="18"/>
       <c r="G59" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H59" s="19"/>
-      <c r="J59" s="17"/>
+      <c r="H59" s="18"/>
+      <c r="J59" s="16"/>
       <c r="M59" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="P59" s="19"/>
-      <c r="R59" s="17"/>
-      <c r="T59" s="19"/>
+      <c r="P59" s="18"/>
+      <c r="R59" s="16"/>
+      <c r="T59" s="18"/>
       <c r="U59" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="V59" s="19" t="s">
+      <c r="V59" s="18" t="s">
         <v>39</v>
       </c>
       <c r="W59" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="X59" s="19" t="s">
+      <c r="X59" s="18" t="s">
         <v>41</v>
       </c>
       <c r="Y59" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="Z59" s="17" t="s">
+      <c r="Z59" s="16" t="s">
         <v>44</v>
       </c>
       <c r="AC59" s="0" t="s">
@@ -2461,8 +2457,8 @@
       <c r="T60" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="V60" s="19"/>
-      <c r="X60" s="19"/>
+      <c r="V60" s="18"/>
+      <c r="X60" s="18"/>
       <c r="AE60" s="0" t="s">
         <v>45</v>
       </c>
@@ -2495,10 +2491,10 @@
       <c r="S61" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="V61" s="19"/>
-      <c r="X61" s="19"/>
-      <c r="AE61" s="19"/>
-      <c r="AG61" s="19"/>
+      <c r="V61" s="18"/>
+      <c r="X61" s="18"/>
+      <c r="AE61" s="18"/>
+      <c r="AG61" s="18"/>
       <c r="AH61" s="0"/>
       <c r="AI61" s="0"/>
       <c r="AJ61" s="8" t="s">
@@ -2519,40 +2515,40 @@
       <c r="A63" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="20"/>
-      <c r="N63" s="20"/>
-      <c r="O63" s="20"/>
-      <c r="P63" s="20"/>
-      <c r="Q63" s="20"/>
-      <c r="R63" s="20"/>
-      <c r="S63" s="20"/>
-      <c r="T63" s="20"/>
-      <c r="U63" s="20"/>
-      <c r="V63" s="20"/>
-      <c r="W63" s="20"/>
-      <c r="X63" s="20"/>
-      <c r="Y63" s="20"/>
-      <c r="Z63" s="20"/>
-      <c r="AA63" s="20"/>
-      <c r="AB63" s="20"/>
-      <c r="AC63" s="20"/>
-      <c r="AD63" s="20"/>
-      <c r="AE63" s="20"/>
-      <c r="AF63" s="20"/>
-      <c r="AG63" s="20"/>
-      <c r="AH63" s="20"/>
-      <c r="AI63" s="20"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="19"/>
+      <c r="Q63" s="19"/>
+      <c r="R63" s="19"/>
+      <c r="S63" s="19"/>
+      <c r="T63" s="19"/>
+      <c r="U63" s="19"/>
+      <c r="V63" s="19"/>
+      <c r="W63" s="19"/>
+      <c r="X63" s="19"/>
+      <c r="Y63" s="19"/>
+      <c r="Z63" s="19"/>
+      <c r="AA63" s="19"/>
+      <c r="AB63" s="19"/>
+      <c r="AC63" s="19"/>
+      <c r="AD63" s="19"/>
+      <c r="AE63" s="19"/>
+      <c r="AF63" s="19"/>
+      <c r="AG63" s="19"/>
+      <c r="AH63" s="19"/>
+      <c r="AI63" s="19"/>
       <c r="AJ63" s="8" t="s">
         <v>27</v>
       </c>
@@ -2593,14 +2589,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16" t="s">
+    <row r="66" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B66" s="2"/>
       <c r="K66" s="2"/>
-      <c r="S66" s="17"/>
-      <c r="AA66" s="17"/>
+      <c r="S66" s="16"/>
+      <c r="AA66" s="16"/>
       <c r="AI66" s="8" t="s">
         <v>27</v>
       </c>
@@ -2669,32 +2665,32 @@
       <c r="A67" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I67" s="19"/>
+      <c r="B67" s="16"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" s="18"/>
       <c r="J67" s="0"/>
-      <c r="K67" s="17" t="s">
+      <c r="K67" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="Q67" s="19"/>
+      <c r="Q67" s="18"/>
       <c r="R67" s="0"/>
-      <c r="S67" s="17" t="s">
+      <c r="S67" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="U67" s="19"/>
+      <c r="U67" s="18"/>
       <c r="W67" s="0" t="s">
         <v>30</v>
       </c>
       <c r="Z67" s="0"/>
-      <c r="AA67" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC67" s="19"/>
-      <c r="AE67" s="19"/>
-      <c r="AG67" s="19"/>
+      <c r="AA67" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="18"/>
+      <c r="AE67" s="18"/>
+      <c r="AG67" s="18"/>
       <c r="AH67" s="0"/>
       <c r="AI67" s="1" t="s">
         <v>27</v>
@@ -2721,7 +2717,7 @@
       <c r="Z68" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AA68" s="17"/>
+      <c r="AA68" s="16"/>
       <c r="AC68" s="0" t="s">
         <v>29</v>
       </c>
@@ -2753,7 +2749,7 @@
       <c r="R69" s="0"/>
       <c r="S69" s="2"/>
       <c r="Z69" s="0"/>
-      <c r="AA69" s="17"/>
+      <c r="AA69" s="16"/>
       <c r="AH69" s="0" t="n">
         <v>0</v>
       </c>
@@ -2782,39 +2778,39 @@
       <c r="A71" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="20"/>
-      <c r="J71" s="20"/>
-      <c r="K71" s="20"/>
-      <c r="L71" s="20"/>
-      <c r="M71" s="20"/>
-      <c r="N71" s="20"/>
-      <c r="O71" s="20"/>
-      <c r="P71" s="20"/>
-      <c r="Q71" s="20"/>
-      <c r="R71" s="20"/>
-      <c r="S71" s="20"/>
-      <c r="T71" s="20"/>
-      <c r="U71" s="20"/>
-      <c r="V71" s="20"/>
-      <c r="W71" s="20"/>
-      <c r="X71" s="20"/>
-      <c r="Y71" s="20"/>
-      <c r="Z71" s="20"/>
-      <c r="AA71" s="20"/>
-      <c r="AB71" s="20"/>
-      <c r="AC71" s="20"/>
-      <c r="AD71" s="20"/>
-      <c r="AE71" s="20"/>
-      <c r="AF71" s="20"/>
-      <c r="AG71" s="20"/>
-      <c r="AH71" s="20"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
+      <c r="K71" s="19"/>
+      <c r="L71" s="19"/>
+      <c r="M71" s="19"/>
+      <c r="N71" s="19"/>
+      <c r="O71" s="19"/>
+      <c r="P71" s="19"/>
+      <c r="Q71" s="19"/>
+      <c r="R71" s="19"/>
+      <c r="S71" s="19"/>
+      <c r="T71" s="19"/>
+      <c r="U71" s="19"/>
+      <c r="V71" s="19"/>
+      <c r="W71" s="19"/>
+      <c r="X71" s="19"/>
+      <c r="Y71" s="19"/>
+      <c r="Z71" s="19"/>
+      <c r="AA71" s="19"/>
+      <c r="AB71" s="19"/>
+      <c r="AC71" s="19"/>
+      <c r="AD71" s="19"/>
+      <c r="AE71" s="19"/>
+      <c r="AF71" s="19"/>
+      <c r="AG71" s="19"/>
+      <c r="AH71" s="19"/>
       <c r="AI71" s="1" t="s">
         <v>27</v>
       </c>
@@ -2849,14 +2845,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="16" t="s">
+    <row r="74" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B74" s="2"/>
       <c r="J74" s="2"/>
-      <c r="R74" s="17"/>
-      <c r="Z74" s="17"/>
+      <c r="R74" s="16"/>
+      <c r="Z74" s="16"/>
       <c r="AH74" s="8" t="s">
         <v>27</v>
       </c>
@@ -2926,7 +2922,7 @@
       <c r="A75" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B75" s="17"/>
+      <c r="B75" s="16"/>
       <c r="D75" s="0" t="n">
         <v>0</v>
       </c>
@@ -2936,17 +2932,17 @@
       <c r="F75" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J75" s="17"/>
-      <c r="P75" s="19"/>
-      <c r="R75" s="17" t="s">
+      <c r="J75" s="16"/>
+      <c r="P75" s="18"/>
+      <c r="R75" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="T75" s="19"/>
-      <c r="V75" s="19" t="s">
+      <c r="T75" s="18"/>
+      <c r="V75" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X75" s="19"/>
-      <c r="Z75" s="17" t="n">
+      <c r="X75" s="18"/>
+      <c r="Z75" s="16" t="n">
         <v>0</v>
       </c>
       <c r="AH75" s="8" t="s">
@@ -2978,8 +2974,8 @@
       <c r="U76" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="V76" s="19"/>
-      <c r="X76" s="19"/>
+      <c r="V76" s="18"/>
+      <c r="X76" s="18"/>
       <c r="Y76" s="0" t="n">
         <v>0</v>
       </c>
@@ -3012,10 +3008,10 @@
       <c r="M77" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="V77" s="19"/>
-      <c r="X77" s="19"/>
-      <c r="AD77" s="19"/>
-      <c r="AF77" s="19"/>
+      <c r="V77" s="18"/>
+      <c r="X77" s="18"/>
+      <c r="AD77" s="18"/>
+      <c r="AF77" s="18"/>
       <c r="AH77" s="8" t="s">
         <v>27</v>
       </c>
@@ -3032,38 +3028,38 @@
       <c r="A79" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="20"/>
-      <c r="H79" s="20"/>
-      <c r="I79" s="20"/>
-      <c r="J79" s="20"/>
-      <c r="K79" s="20"/>
-      <c r="L79" s="20"/>
-      <c r="M79" s="20"/>
-      <c r="N79" s="20"/>
-      <c r="O79" s="20"/>
-      <c r="P79" s="20"/>
-      <c r="Q79" s="20"/>
-      <c r="R79" s="20"/>
-      <c r="S79" s="20"/>
-      <c r="T79" s="20"/>
-      <c r="U79" s="20"/>
-      <c r="V79" s="20"/>
-      <c r="W79" s="20"/>
-      <c r="X79" s="20"/>
-      <c r="Y79" s="20"/>
-      <c r="Z79" s="20"/>
-      <c r="AA79" s="20"/>
-      <c r="AB79" s="20"/>
-      <c r="AC79" s="20"/>
-      <c r="AD79" s="20"/>
-      <c r="AE79" s="20"/>
-      <c r="AF79" s="20"/>
-      <c r="AG79" s="20"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="19"/>
+      <c r="L79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="19"/>
+      <c r="O79" s="19"/>
+      <c r="P79" s="19"/>
+      <c r="Q79" s="19"/>
+      <c r="R79" s="19"/>
+      <c r="S79" s="19"/>
+      <c r="T79" s="19"/>
+      <c r="U79" s="19"/>
+      <c r="V79" s="19"/>
+      <c r="W79" s="19"/>
+      <c r="X79" s="19"/>
+      <c r="Y79" s="19"/>
+      <c r="Z79" s="19"/>
+      <c r="AA79" s="19"/>
+      <c r="AB79" s="19"/>
+      <c r="AC79" s="19"/>
+      <c r="AD79" s="19"/>
+      <c r="AE79" s="19"/>
+      <c r="AF79" s="19"/>
+      <c r="AG79" s="19"/>
       <c r="AH79" s="8" t="s">
         <v>27</v>
       </c>
@@ -3092,14 +3088,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="16" t="s">
+    <row r="82" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B82" s="2"/>
       <c r="J82" s="2"/>
-      <c r="R82" s="17"/>
-      <c r="Z82" s="17"/>
+      <c r="R82" s="16"/>
+      <c r="Z82" s="16"/>
       <c r="AH82" s="8" t="s">
         <v>27</v>
       </c>
@@ -3171,38 +3167,38 @@
       <c r="A83" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B83" s="17"/>
+      <c r="B83" s="16"/>
       <c r="D83" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F83" s="19" t="s">
+      <c r="F83" s="18" t="s">
         <v>39</v>
       </c>
       <c r="G83" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="H83" s="19" t="s">
+      <c r="H83" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J83" s="17" t="n">
+      <c r="J83" s="16" t="n">
         <v>0</v>
       </c>
       <c r="N83" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="P83" s="19"/>
-      <c r="R83" s="17" t="s">
+      <c r="P83" s="18"/>
+      <c r="R83" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="T83" s="19"/>
-      <c r="V83" s="19" t="s">
+      <c r="T83" s="18"/>
+      <c r="V83" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X83" s="19"/>
-      <c r="Z83" s="17" t="n">
+      <c r="X83" s="18"/>
+      <c r="Z83" s="16" t="n">
         <v>0</v>
       </c>
       <c r="AH83" s="8" t="s">
@@ -3228,8 +3224,8 @@
       <c r="U84" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="V84" s="19"/>
-      <c r="X84" s="19"/>
+      <c r="V84" s="18"/>
+      <c r="X84" s="18"/>
       <c r="Y84" s="0" t="n">
         <v>0</v>
       </c>
@@ -3259,10 +3255,10 @@
       <c r="M85" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="V85" s="19"/>
-      <c r="X85" s="19"/>
-      <c r="AD85" s="19"/>
-      <c r="AF85" s="19"/>
+      <c r="V85" s="18"/>
+      <c r="X85" s="18"/>
+      <c r="AD85" s="18"/>
+      <c r="AF85" s="18"/>
       <c r="AG85" s="0" t="n">
         <v>0</v>
       </c>
@@ -3282,38 +3278,38 @@
       <c r="A87" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="20"/>
-      <c r="H87" s="20"/>
-      <c r="I87" s="20"/>
-      <c r="J87" s="20"/>
-      <c r="K87" s="20"/>
-      <c r="L87" s="20"/>
-      <c r="M87" s="20"/>
-      <c r="N87" s="20"/>
-      <c r="O87" s="20"/>
-      <c r="P87" s="20"/>
-      <c r="Q87" s="20"/>
-      <c r="R87" s="20"/>
-      <c r="S87" s="20"/>
-      <c r="T87" s="20"/>
-      <c r="U87" s="20"/>
-      <c r="V87" s="20"/>
-      <c r="W87" s="20"/>
-      <c r="X87" s="20"/>
-      <c r="Y87" s="20"/>
-      <c r="Z87" s="20"/>
-      <c r="AA87" s="20"/>
-      <c r="AB87" s="20"/>
-      <c r="AC87" s="20"/>
-      <c r="AD87" s="20"/>
-      <c r="AE87" s="20"/>
-      <c r="AF87" s="20"/>
-      <c r="AG87" s="20"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="19"/>
+      <c r="L87" s="19"/>
+      <c r="M87" s="19"/>
+      <c r="N87" s="19"/>
+      <c r="O87" s="19"/>
+      <c r="P87" s="19"/>
+      <c r="Q87" s="19"/>
+      <c r="R87" s="19"/>
+      <c r="S87" s="19"/>
+      <c r="T87" s="19"/>
+      <c r="U87" s="19"/>
+      <c r="V87" s="19"/>
+      <c r="W87" s="19"/>
+      <c r="X87" s="19"/>
+      <c r="Y87" s="19"/>
+      <c r="Z87" s="19"/>
+      <c r="AA87" s="19"/>
+      <c r="AB87" s="19"/>
+      <c r="AC87" s="19"/>
+      <c r="AD87" s="19"/>
+      <c r="AE87" s="19"/>
+      <c r="AF87" s="19"/>
+      <c r="AG87" s="19"/>
       <c r="AH87" s="8" t="s">
         <v>27</v>
       </c>
@@ -3345,14 +3341,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="16" t="s">
+    <row r="90" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B90" s="2"/>
       <c r="J90" s="2"/>
-      <c r="R90" s="17"/>
-      <c r="Z90" s="17"/>
+      <c r="R90" s="16"/>
+      <c r="Z90" s="16"/>
       <c r="AH90" s="8" t="s">
         <v>27</v>
       </c>
@@ -3422,28 +3418,28 @@
       <c r="A91" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B91" s="17"/>
+      <c r="B91" s="16"/>
       <c r="D91" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E91" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F91" s="19" t="s">
+      <c r="F91" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H91" s="19"/>
-      <c r="J91" s="17"/>
-      <c r="P91" s="19"/>
-      <c r="R91" s="17" t="s">
+      <c r="H91" s="18"/>
+      <c r="J91" s="16"/>
+      <c r="P91" s="18"/>
+      <c r="R91" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="T91" s="19"/>
-      <c r="V91" s="19" t="s">
+      <c r="T91" s="18"/>
+      <c r="V91" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X91" s="19"/>
-      <c r="Z91" s="17" t="n">
+      <c r="X91" s="18"/>
+      <c r="Z91" s="16" t="n">
         <v>0</v>
       </c>
       <c r="AH91" s="8" t="s">
@@ -3475,8 +3471,8 @@
       <c r="U92" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="V92" s="19"/>
-      <c r="X92" s="19"/>
+      <c r="V92" s="18"/>
+      <c r="X92" s="18"/>
       <c r="Y92" s="0" t="n">
         <v>0</v>
       </c>
@@ -3509,10 +3505,10 @@
       <c r="M93" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="V93" s="19"/>
-      <c r="X93" s="19"/>
-      <c r="AD93" s="19"/>
-      <c r="AF93" s="19"/>
+      <c r="V93" s="18"/>
+      <c r="X93" s="18"/>
+      <c r="AD93" s="18"/>
+      <c r="AF93" s="18"/>
       <c r="AH93" s="8" t="s">
         <v>27</v>
       </c>
@@ -3529,38 +3525,38 @@
       <c r="A95" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
-      <c r="H95" s="20"/>
-      <c r="I95" s="20"/>
-      <c r="J95" s="20"/>
-      <c r="K95" s="20"/>
-      <c r="L95" s="20"/>
-      <c r="M95" s="20"/>
-      <c r="N95" s="20"/>
-      <c r="O95" s="20"/>
-      <c r="P95" s="20"/>
-      <c r="Q95" s="20"/>
-      <c r="R95" s="20"/>
-      <c r="S95" s="20"/>
-      <c r="T95" s="20"/>
-      <c r="U95" s="20"/>
-      <c r="V95" s="20"/>
-      <c r="W95" s="20"/>
-      <c r="X95" s="20"/>
-      <c r="Y95" s="20"/>
-      <c r="Z95" s="20"/>
-      <c r="AA95" s="20"/>
-      <c r="AB95" s="20"/>
-      <c r="AC95" s="20"/>
-      <c r="AD95" s="20"/>
-      <c r="AE95" s="20"/>
-      <c r="AF95" s="20"/>
-      <c r="AG95" s="20"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="19"/>
+      <c r="I95" s="19"/>
+      <c r="J95" s="19"/>
+      <c r="K95" s="19"/>
+      <c r="L95" s="19"/>
+      <c r="M95" s="19"/>
+      <c r="N95" s="19"/>
+      <c r="O95" s="19"/>
+      <c r="P95" s="19"/>
+      <c r="Q95" s="19"/>
+      <c r="R95" s="19"/>
+      <c r="S95" s="19"/>
+      <c r="T95" s="19"/>
+      <c r="U95" s="19"/>
+      <c r="V95" s="19"/>
+      <c r="W95" s="19"/>
+      <c r="X95" s="19"/>
+      <c r="Y95" s="19"/>
+      <c r="Z95" s="19"/>
+      <c r="AA95" s="19"/>
+      <c r="AB95" s="19"/>
+      <c r="AC95" s="19"/>
+      <c r="AD95" s="19"/>
+      <c r="AE95" s="19"/>
+      <c r="AF95" s="19"/>
+      <c r="AG95" s="19"/>
       <c r="AH95" s="8" t="s">
         <v>27</v>
       </c>
@@ -3589,14 +3585,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="16" t="s">
+    <row r="98" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B98" s="2"/>
       <c r="J98" s="2"/>
-      <c r="R98" s="17"/>
-      <c r="Z98" s="21" t="s">
+      <c r="R98" s="16"/>
+      <c r="Z98" s="20" t="s">
         <v>27</v>
       </c>
       <c r="AH98" s="8"/>
@@ -3666,33 +3662,33 @@
       <c r="A99" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B99" s="17"/>
+      <c r="B99" s="16"/>
       <c r="D99" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E99" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="F99" s="19" t="s">
+      <c r="F99" s="18" t="s">
         <v>39</v>
       </c>
       <c r="G99" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="H99" s="19" t="s">
+      <c r="H99" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J99" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="P99" s="19"/>
-      <c r="R99" s="17" t="s">
+      <c r="J99" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P99" s="18"/>
+      <c r="R99" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="T99" s="19"/>
-      <c r="V99" s="19"/>
-      <c r="X99" s="19"/>
-      <c r="Z99" s="21" t="s">
+      <c r="T99" s="18"/>
+      <c r="V99" s="18"/>
+      <c r="X99" s="18"/>
+      <c r="Z99" s="20" t="s">
         <v>27</v>
       </c>
       <c r="AH99" s="8"/>
@@ -3707,8 +3703,8 @@
       <c r="I100" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="V100" s="19"/>
-      <c r="X100" s="19"/>
+      <c r="V100" s="18"/>
+      <c r="X100" s="18"/>
       <c r="Z100" s="2" t="s">
         <v>27</v>
       </c>
@@ -3721,13 +3717,13 @@
       <c r="B101" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V101" s="19"/>
-      <c r="X101" s="19"/>
+      <c r="V101" s="18"/>
+      <c r="X101" s="18"/>
       <c r="Z101" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD101" s="19"/>
-      <c r="AF101" s="19"/>
+      <c r="AD101" s="18"/>
+      <c r="AF101" s="18"/>
       <c r="AH101" s="8"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,40 +3739,40 @@
       <c r="A103" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B103" s="20"/>
-      <c r="C103" s="20"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="20"/>
-      <c r="H103" s="20"/>
-      <c r="I103" s="20"/>
-      <c r="J103" s="20"/>
-      <c r="K103" s="20"/>
-      <c r="L103" s="20"/>
-      <c r="M103" s="20"/>
-      <c r="N103" s="20"/>
-      <c r="O103" s="20"/>
-      <c r="P103" s="20"/>
-      <c r="Q103" s="20"/>
-      <c r="R103" s="20"/>
-      <c r="S103" s="20"/>
-      <c r="T103" s="20"/>
-      <c r="U103" s="20"/>
-      <c r="V103" s="20"/>
-      <c r="W103" s="20"/>
-      <c r="X103" s="20"/>
-      <c r="Y103" s="20"/>
-      <c r="Z103" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA103" s="20"/>
-      <c r="AB103" s="20"/>
-      <c r="AC103" s="20"/>
-      <c r="AD103" s="20"/>
-      <c r="AE103" s="20"/>
-      <c r="AF103" s="20"/>
-      <c r="AG103" s="20"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+      <c r="J103" s="19"/>
+      <c r="K103" s="19"/>
+      <c r="L103" s="19"/>
+      <c r="M103" s="19"/>
+      <c r="N103" s="19"/>
+      <c r="O103" s="19"/>
+      <c r="P103" s="19"/>
+      <c r="Q103" s="19"/>
+      <c r="R103" s="19"/>
+      <c r="S103" s="19"/>
+      <c r="T103" s="19"/>
+      <c r="U103" s="19"/>
+      <c r="V103" s="19"/>
+      <c r="W103" s="19"/>
+      <c r="X103" s="19"/>
+      <c r="Y103" s="19"/>
+      <c r="Z103" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA103" s="19"/>
+      <c r="AB103" s="19"/>
+      <c r="AC103" s="19"/>
+      <c r="AD103" s="19"/>
+      <c r="AE103" s="19"/>
+      <c r="AF103" s="19"/>
+      <c r="AG103" s="19"/>
       <c r="AH103" s="8"/>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3803,11 +3799,11 @@
       </c>
       <c r="AH105" s="8"/>
     </row>
-    <row r="106" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2"/>
       <c r="J106" s="2"/>
-      <c r="R106" s="17"/>
-      <c r="Z106" s="17"/>
+      <c r="R106" s="16"/>
+      <c r="Z106" s="16"/>
       <c r="AH106" s="8"/>
       <c r="AI106" s="1"/>
       <c r="AJ106" s="1"/>
@@ -3873,30 +3869,30 @@
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8"/>
-      <c r="B107" s="17"/>
-      <c r="F107" s="19"/>
-      <c r="H107" s="19"/>
-      <c r="J107" s="17"/>
-      <c r="P107" s="19"/>
-      <c r="R107" s="17"/>
-      <c r="T107" s="19"/>
-      <c r="V107" s="19"/>
-      <c r="X107" s="19"/>
-      <c r="Z107" s="17"/>
+      <c r="B107" s="16"/>
+      <c r="F107" s="18"/>
+      <c r="H107" s="18"/>
+      <c r="J107" s="16"/>
+      <c r="P107" s="18"/>
+      <c r="R107" s="16"/>
+      <c r="T107" s="18"/>
+      <c r="V107" s="18"/>
+      <c r="X107" s="18"/>
+      <c r="Z107" s="16"/>
       <c r="AH107" s="8"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8"/>
-      <c r="V108" s="19"/>
-      <c r="X108" s="19"/>
+      <c r="V108" s="18"/>
+      <c r="X108" s="18"/>
       <c r="AH108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8"/>
-      <c r="V109" s="19"/>
-      <c r="X109" s="19"/>
-      <c r="AD109" s="19"/>
-      <c r="AF109" s="19"/>
+      <c r="V109" s="18"/>
+      <c r="X109" s="18"/>
+      <c r="AD109" s="18"/>
+      <c r="AF109" s="18"/>
       <c r="AH109" s="8"/>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,38 +3901,38 @@
     </row>
     <row r="111" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="8"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="20"/>
-      <c r="D111" s="20"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="20"/>
-      <c r="J111" s="20"/>
-      <c r="K111" s="20"/>
-      <c r="L111" s="20"/>
-      <c r="M111" s="20"/>
-      <c r="N111" s="20"/>
-      <c r="O111" s="20"/>
-      <c r="P111" s="20"/>
-      <c r="Q111" s="20"/>
-      <c r="R111" s="20"/>
-      <c r="S111" s="20"/>
-      <c r="T111" s="20"/>
-      <c r="U111" s="20"/>
-      <c r="V111" s="20"/>
-      <c r="W111" s="20"/>
-      <c r="X111" s="20"/>
-      <c r="Y111" s="20"/>
-      <c r="Z111" s="20"/>
-      <c r="AA111" s="20"/>
-      <c r="AB111" s="20"/>
-      <c r="AC111" s="20"/>
-      <c r="AD111" s="20"/>
-      <c r="AE111" s="20"/>
-      <c r="AF111" s="20"/>
-      <c r="AG111" s="20"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="19"/>
+      <c r="I111" s="19"/>
+      <c r="J111" s="19"/>
+      <c r="K111" s="19"/>
+      <c r="L111" s="19"/>
+      <c r="M111" s="19"/>
+      <c r="N111" s="19"/>
+      <c r="O111" s="19"/>
+      <c r="P111" s="19"/>
+      <c r="Q111" s="19"/>
+      <c r="R111" s="19"/>
+      <c r="S111" s="19"/>
+      <c r="T111" s="19"/>
+      <c r="U111" s="19"/>
+      <c r="V111" s="19"/>
+      <c r="W111" s="19"/>
+      <c r="X111" s="19"/>
+      <c r="Y111" s="19"/>
+      <c r="Z111" s="19"/>
+      <c r="AA111" s="19"/>
+      <c r="AB111" s="19"/>
+      <c r="AC111" s="19"/>
+      <c r="AD111" s="19"/>
+      <c r="AE111" s="19"/>
+      <c r="AF111" s="19"/>
+      <c r="AG111" s="19"/>
       <c r="AH111" s="8"/>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,11 +3951,11 @@
       <c r="Z113" s="2"/>
       <c r="AH113" s="8"/>
     </row>
-    <row r="114" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2"/>
       <c r="J114" s="2"/>
-      <c r="R114" s="17"/>
-      <c r="Z114" s="17"/>
+      <c r="R114" s="16"/>
+      <c r="Z114" s="16"/>
       <c r="AH114" s="8"/>
       <c r="AI114" s="1"/>
       <c r="AJ114" s="1"/>
@@ -4025,30 +4021,30 @@
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="8"/>
-      <c r="B115" s="17"/>
-      <c r="F115" s="19"/>
-      <c r="H115" s="19"/>
-      <c r="J115" s="17"/>
-      <c r="P115" s="19"/>
-      <c r="R115" s="17"/>
-      <c r="T115" s="19"/>
-      <c r="V115" s="19"/>
-      <c r="X115" s="19"/>
-      <c r="Z115" s="17"/>
+      <c r="B115" s="16"/>
+      <c r="F115" s="18"/>
+      <c r="H115" s="18"/>
+      <c r="J115" s="16"/>
+      <c r="P115" s="18"/>
+      <c r="R115" s="16"/>
+      <c r="T115" s="18"/>
+      <c r="V115" s="18"/>
+      <c r="X115" s="18"/>
+      <c r="Z115" s="16"/>
       <c r="AH115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8"/>
-      <c r="V116" s="19"/>
-      <c r="X116" s="19"/>
+      <c r="V116" s="18"/>
+      <c r="X116" s="18"/>
       <c r="AH116" s="8"/>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8"/>
-      <c r="V117" s="19"/>
-      <c r="X117" s="19"/>
-      <c r="AD117" s="19"/>
-      <c r="AF117" s="19"/>
+      <c r="V117" s="18"/>
+      <c r="X117" s="18"/>
+      <c r="AD117" s="18"/>
+      <c r="AF117" s="18"/>
       <c r="AH117" s="8"/>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4057,38 +4053,38 @@
     </row>
     <row r="119" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="8"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="20"/>
-      <c r="D119" s="20"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="20"/>
-      <c r="H119" s="20"/>
-      <c r="I119" s="20"/>
-      <c r="J119" s="20"/>
-      <c r="K119" s="20"/>
-      <c r="L119" s="20"/>
-      <c r="M119" s="20"/>
-      <c r="N119" s="20"/>
-      <c r="O119" s="20"/>
-      <c r="P119" s="20"/>
-      <c r="Q119" s="20"/>
-      <c r="R119" s="20"/>
-      <c r="S119" s="20"/>
-      <c r="T119" s="20"/>
-      <c r="U119" s="20"/>
-      <c r="V119" s="20"/>
-      <c r="W119" s="20"/>
-      <c r="X119" s="20"/>
-      <c r="Y119" s="20"/>
-      <c r="Z119" s="20"/>
-      <c r="AA119" s="20"/>
-      <c r="AB119" s="20"/>
-      <c r="AC119" s="20"/>
-      <c r="AD119" s="20"/>
-      <c r="AE119" s="20"/>
-      <c r="AF119" s="20"/>
-      <c r="AG119" s="20"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="19"/>
+      <c r="I119" s="19"/>
+      <c r="J119" s="19"/>
+      <c r="K119" s="19"/>
+      <c r="L119" s="19"/>
+      <c r="M119" s="19"/>
+      <c r="N119" s="19"/>
+      <c r="O119" s="19"/>
+      <c r="P119" s="19"/>
+      <c r="Q119" s="19"/>
+      <c r="R119" s="19"/>
+      <c r="S119" s="19"/>
+      <c r="T119" s="19"/>
+      <c r="U119" s="19"/>
+      <c r="V119" s="19"/>
+      <c r="W119" s="19"/>
+      <c r="X119" s="19"/>
+      <c r="Y119" s="19"/>
+      <c r="Z119" s="19"/>
+      <c r="AA119" s="19"/>
+      <c r="AB119" s="19"/>
+      <c r="AC119" s="19"/>
+      <c r="AD119" s="19"/>
+      <c r="AE119" s="19"/>
+      <c r="AF119" s="19"/>
+      <c r="AG119" s="19"/>
       <c r="AH119" s="8"/>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4107,11 +4103,11 @@
       <c r="Z121" s="2"/>
       <c r="AH121" s="8"/>
     </row>
-    <row r="122" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2"/>
       <c r="J122" s="2"/>
-      <c r="R122" s="17"/>
-      <c r="Z122" s="17"/>
+      <c r="R122" s="16"/>
+      <c r="Z122" s="16"/>
       <c r="AH122" s="8"/>
       <c r="AI122" s="1"/>
       <c r="AJ122" s="1"/>
@@ -4177,30 +4173,30 @@
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="8"/>
-      <c r="B123" s="17"/>
-      <c r="F123" s="19"/>
-      <c r="H123" s="19"/>
-      <c r="J123" s="17"/>
-      <c r="P123" s="19"/>
-      <c r="R123" s="17"/>
-      <c r="T123" s="19"/>
-      <c r="V123" s="19"/>
-      <c r="X123" s="19"/>
-      <c r="Z123" s="17"/>
+      <c r="B123" s="16"/>
+      <c r="F123" s="18"/>
+      <c r="H123" s="18"/>
+      <c r="J123" s="16"/>
+      <c r="P123" s="18"/>
+      <c r="R123" s="16"/>
+      <c r="T123" s="18"/>
+      <c r="V123" s="18"/>
+      <c r="X123" s="18"/>
+      <c r="Z123" s="16"/>
       <c r="AH123" s="8"/>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="8"/>
-      <c r="V124" s="19"/>
-      <c r="X124" s="19"/>
+      <c r="V124" s="18"/>
+      <c r="X124" s="18"/>
       <c r="AH124" s="8"/>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8"/>
-      <c r="V125" s="19"/>
-      <c r="X125" s="19"/>
-      <c r="AD125" s="19"/>
-      <c r="AF125" s="19"/>
+      <c r="V125" s="18"/>
+      <c r="X125" s="18"/>
+      <c r="AD125" s="18"/>
+      <c r="AF125" s="18"/>
       <c r="AH125" s="8"/>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4209,38 +4205,38 @@
     </row>
     <row r="127" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="8"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="20"/>
-      <c r="D127" s="20"/>
-      <c r="E127" s="20"/>
-      <c r="F127" s="20"/>
-      <c r="G127" s="20"/>
-      <c r="H127" s="20"/>
-      <c r="I127" s="20"/>
-      <c r="J127" s="20"/>
-      <c r="K127" s="20"/>
-      <c r="L127" s="20"/>
-      <c r="M127" s="20"/>
-      <c r="N127" s="20"/>
-      <c r="O127" s="20"/>
-      <c r="P127" s="20"/>
-      <c r="Q127" s="20"/>
-      <c r="R127" s="20"/>
-      <c r="S127" s="20"/>
-      <c r="T127" s="20"/>
-      <c r="U127" s="20"/>
-      <c r="V127" s="20"/>
-      <c r="W127" s="20"/>
-      <c r="X127" s="20"/>
-      <c r="Y127" s="20"/>
-      <c r="Z127" s="20"/>
-      <c r="AA127" s="20"/>
-      <c r="AB127" s="20"/>
-      <c r="AC127" s="20"/>
-      <c r="AD127" s="20"/>
-      <c r="AE127" s="20"/>
-      <c r="AF127" s="20"/>
-      <c r="AG127" s="20"/>
+      <c r="B127" s="19"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="19"/>
+      <c r="G127" s="19"/>
+      <c r="H127" s="19"/>
+      <c r="I127" s="19"/>
+      <c r="J127" s="19"/>
+      <c r="K127" s="19"/>
+      <c r="L127" s="19"/>
+      <c r="M127" s="19"/>
+      <c r="N127" s="19"/>
+      <c r="O127" s="19"/>
+      <c r="P127" s="19"/>
+      <c r="Q127" s="19"/>
+      <c r="R127" s="19"/>
+      <c r="S127" s="19"/>
+      <c r="T127" s="19"/>
+      <c r="U127" s="19"/>
+      <c r="V127" s="19"/>
+      <c r="W127" s="19"/>
+      <c r="X127" s="19"/>
+      <c r="Y127" s="19"/>
+      <c r="Z127" s="19"/>
+      <c r="AA127" s="19"/>
+      <c r="AB127" s="19"/>
+      <c r="AC127" s="19"/>
+      <c r="AD127" s="19"/>
+      <c r="AE127" s="19"/>
+      <c r="AF127" s="19"/>
+      <c r="AG127" s="19"/>
       <c r="AH127" s="8"/>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4259,11 +4255,11 @@
       <c r="Z129" s="2"/>
       <c r="AH129" s="8"/>
     </row>
-    <row r="130" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2"/>
       <c r="J130" s="2"/>
-      <c r="R130" s="17"/>
-      <c r="Z130" s="17"/>
+      <c r="R130" s="16"/>
+      <c r="Z130" s="16"/>
       <c r="AH130" s="8"/>
       <c r="AI130" s="1"/>
       <c r="AJ130" s="1"/>
@@ -4329,30 +4325,30 @@
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="8"/>
-      <c r="B131" s="17"/>
-      <c r="F131" s="19"/>
-      <c r="H131" s="19"/>
-      <c r="J131" s="17"/>
-      <c r="P131" s="19"/>
-      <c r="R131" s="17"/>
-      <c r="T131" s="19"/>
-      <c r="V131" s="19"/>
-      <c r="X131" s="19"/>
-      <c r="Z131" s="17"/>
+      <c r="B131" s="16"/>
+      <c r="F131" s="18"/>
+      <c r="H131" s="18"/>
+      <c r="J131" s="16"/>
+      <c r="P131" s="18"/>
+      <c r="R131" s="16"/>
+      <c r="T131" s="18"/>
+      <c r="V131" s="18"/>
+      <c r="X131" s="18"/>
+      <c r="Z131" s="16"/>
       <c r="AH131" s="8"/>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="8"/>
-      <c r="V132" s="19"/>
-      <c r="X132" s="19"/>
+      <c r="V132" s="18"/>
+      <c r="X132" s="18"/>
       <c r="AH132" s="8"/>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="8"/>
-      <c r="V133" s="19"/>
-      <c r="X133" s="19"/>
-      <c r="AD133" s="19"/>
-      <c r="AF133" s="19"/>
+      <c r="V133" s="18"/>
+      <c r="X133" s="18"/>
+      <c r="AD133" s="18"/>
+      <c r="AF133" s="18"/>
       <c r="AH133" s="8"/>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4361,38 +4357,38 @@
     </row>
     <row r="135" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="8"/>
-      <c r="B135" s="20"/>
-      <c r="C135" s="20"/>
-      <c r="D135" s="20"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="20"/>
-      <c r="G135" s="20"/>
-      <c r="H135" s="20"/>
-      <c r="I135" s="20"/>
-      <c r="J135" s="20"/>
-      <c r="K135" s="20"/>
-      <c r="L135" s="20"/>
-      <c r="M135" s="20"/>
-      <c r="N135" s="20"/>
-      <c r="O135" s="20"/>
-      <c r="P135" s="20"/>
-      <c r="Q135" s="20"/>
-      <c r="R135" s="20"/>
-      <c r="S135" s="20"/>
-      <c r="T135" s="20"/>
-      <c r="U135" s="20"/>
-      <c r="V135" s="20"/>
-      <c r="W135" s="20"/>
-      <c r="X135" s="20"/>
-      <c r="Y135" s="20"/>
-      <c r="Z135" s="20"/>
-      <c r="AA135" s="20"/>
-      <c r="AB135" s="20"/>
-      <c r="AC135" s="20"/>
-      <c r="AD135" s="20"/>
-      <c r="AE135" s="20"/>
-      <c r="AF135" s="20"/>
-      <c r="AG135" s="20"/>
+      <c r="B135" s="19"/>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="19"/>
+      <c r="G135" s="19"/>
+      <c r="H135" s="19"/>
+      <c r="I135" s="19"/>
+      <c r="J135" s="19"/>
+      <c r="K135" s="19"/>
+      <c r="L135" s="19"/>
+      <c r="M135" s="19"/>
+      <c r="N135" s="19"/>
+      <c r="O135" s="19"/>
+      <c r="P135" s="19"/>
+      <c r="Q135" s="19"/>
+      <c r="R135" s="19"/>
+      <c r="S135" s="19"/>
+      <c r="T135" s="19"/>
+      <c r="U135" s="19"/>
+      <c r="V135" s="19"/>
+      <c r="W135" s="19"/>
+      <c r="X135" s="19"/>
+      <c r="Y135" s="19"/>
+      <c r="Z135" s="19"/>
+      <c r="AA135" s="19"/>
+      <c r="AB135" s="19"/>
+      <c r="AC135" s="19"/>
+      <c r="AD135" s="19"/>
+      <c r="AE135" s="19"/>
+      <c r="AF135" s="19"/>
+      <c r="AG135" s="19"/>
       <c r="AH135" s="8"/>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4411,11 +4407,11 @@
       <c r="Z137" s="2"/>
       <c r="AH137" s="8"/>
     </row>
-    <row r="138" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2"/>
       <c r="J138" s="2"/>
-      <c r="R138" s="17"/>
-      <c r="Z138" s="17"/>
+      <c r="R138" s="16"/>
+      <c r="Z138" s="16"/>
       <c r="AH138" s="8"/>
       <c r="AI138" s="1"/>
       <c r="AJ138" s="1"/>
@@ -4481,30 +4477,30 @@
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8"/>
-      <c r="B139" s="17"/>
-      <c r="F139" s="19"/>
-      <c r="H139" s="19"/>
-      <c r="J139" s="17"/>
-      <c r="P139" s="19"/>
-      <c r="R139" s="17"/>
-      <c r="T139" s="19"/>
-      <c r="V139" s="19"/>
-      <c r="X139" s="19"/>
-      <c r="Z139" s="17"/>
+      <c r="B139" s="16"/>
+      <c r="F139" s="18"/>
+      <c r="H139" s="18"/>
+      <c r="J139" s="16"/>
+      <c r="P139" s="18"/>
+      <c r="R139" s="16"/>
+      <c r="T139" s="18"/>
+      <c r="V139" s="18"/>
+      <c r="X139" s="18"/>
+      <c r="Z139" s="16"/>
       <c r="AH139" s="8"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="8"/>
-      <c r="V140" s="19"/>
-      <c r="X140" s="19"/>
+      <c r="V140" s="18"/>
+      <c r="X140" s="18"/>
       <c r="AH140" s="8"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8"/>
-      <c r="V141" s="19"/>
-      <c r="X141" s="19"/>
-      <c r="AD141" s="19"/>
-      <c r="AF141" s="19"/>
+      <c r="V141" s="18"/>
+      <c r="X141" s="18"/>
+      <c r="AD141" s="18"/>
+      <c r="AF141" s="18"/>
       <c r="AH141" s="8"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4513,38 +4509,38 @@
     </row>
     <row r="143" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="8"/>
-      <c r="B143" s="20"/>
-      <c r="C143" s="20"/>
-      <c r="D143" s="20"/>
-      <c r="E143" s="20"/>
-      <c r="F143" s="20"/>
-      <c r="G143" s="20"/>
-      <c r="H143" s="20"/>
-      <c r="I143" s="20"/>
-      <c r="J143" s="20"/>
-      <c r="K143" s="20"/>
-      <c r="L143" s="20"/>
-      <c r="M143" s="20"/>
-      <c r="N143" s="20"/>
-      <c r="O143" s="20"/>
-      <c r="P143" s="20"/>
-      <c r="Q143" s="20"/>
-      <c r="R143" s="20"/>
-      <c r="S143" s="20"/>
-      <c r="T143" s="20"/>
-      <c r="U143" s="20"/>
-      <c r="V143" s="20"/>
-      <c r="W143" s="20"/>
-      <c r="X143" s="20"/>
-      <c r="Y143" s="20"/>
-      <c r="Z143" s="20"/>
-      <c r="AA143" s="20"/>
-      <c r="AB143" s="20"/>
-      <c r="AC143" s="20"/>
-      <c r="AD143" s="20"/>
-      <c r="AE143" s="20"/>
-      <c r="AF143" s="20"/>
-      <c r="AG143" s="20"/>
+      <c r="B143" s="19"/>
+      <c r="C143" s="19"/>
+      <c r="D143" s="19"/>
+      <c r="E143" s="19"/>
+      <c r="F143" s="19"/>
+      <c r="G143" s="19"/>
+      <c r="H143" s="19"/>
+      <c r="I143" s="19"/>
+      <c r="J143" s="19"/>
+      <c r="K143" s="19"/>
+      <c r="L143" s="19"/>
+      <c r="M143" s="19"/>
+      <c r="N143" s="19"/>
+      <c r="O143" s="19"/>
+      <c r="P143" s="19"/>
+      <c r="Q143" s="19"/>
+      <c r="R143" s="19"/>
+      <c r="S143" s="19"/>
+      <c r="T143" s="19"/>
+      <c r="U143" s="19"/>
+      <c r="V143" s="19"/>
+      <c r="W143" s="19"/>
+      <c r="X143" s="19"/>
+      <c r="Y143" s="19"/>
+      <c r="Z143" s="19"/>
+      <c r="AA143" s="19"/>
+      <c r="AB143" s="19"/>
+      <c r="AC143" s="19"/>
+      <c r="AD143" s="19"/>
+      <c r="AE143" s="19"/>
+      <c r="AF143" s="19"/>
+      <c r="AG143" s="19"/>
       <c r="AH143" s="8"/>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4563,11 +4559,11 @@
       <c r="Z145" s="2"/>
       <c r="AH145" s="8"/>
     </row>
-    <row r="146" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2"/>
       <c r="J146" s="2"/>
-      <c r="R146" s="17"/>
-      <c r="Z146" s="17"/>
+      <c r="R146" s="16"/>
+      <c r="Z146" s="16"/>
       <c r="AH146" s="8"/>
       <c r="AI146" s="1"/>
       <c r="AJ146" s="1"/>
@@ -4633,30 +4629,30 @@
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="8"/>
-      <c r="B147" s="17"/>
-      <c r="F147" s="19"/>
-      <c r="H147" s="19"/>
-      <c r="J147" s="17"/>
-      <c r="P147" s="19"/>
-      <c r="R147" s="17"/>
-      <c r="T147" s="19"/>
-      <c r="V147" s="19"/>
-      <c r="X147" s="19"/>
-      <c r="Z147" s="17"/>
+      <c r="B147" s="16"/>
+      <c r="F147" s="18"/>
+      <c r="H147" s="18"/>
+      <c r="J147" s="16"/>
+      <c r="P147" s="18"/>
+      <c r="R147" s="16"/>
+      <c r="T147" s="18"/>
+      <c r="V147" s="18"/>
+      <c r="X147" s="18"/>
+      <c r="Z147" s="16"/>
       <c r="AH147" s="8"/>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="8"/>
-      <c r="V148" s="19"/>
-      <c r="X148" s="19"/>
+      <c r="V148" s="18"/>
+      <c r="X148" s="18"/>
       <c r="AH148" s="8"/>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="8"/>
-      <c r="V149" s="19"/>
-      <c r="X149" s="19"/>
-      <c r="AD149" s="19"/>
-      <c r="AF149" s="19"/>
+      <c r="V149" s="18"/>
+      <c r="X149" s="18"/>
+      <c r="AD149" s="18"/>
+      <c r="AF149" s="18"/>
       <c r="AH149" s="8"/>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4665,38 +4661,38 @@
     </row>
     <row r="151" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="8"/>
-      <c r="B151" s="20"/>
-      <c r="C151" s="20"/>
-      <c r="D151" s="20"/>
-      <c r="E151" s="20"/>
-      <c r="F151" s="20"/>
-      <c r="G151" s="20"/>
-      <c r="H151" s="20"/>
-      <c r="I151" s="20"/>
-      <c r="J151" s="20"/>
-      <c r="K151" s="20"/>
-      <c r="L151" s="20"/>
-      <c r="M151" s="20"/>
-      <c r="N151" s="20"/>
-      <c r="O151" s="20"/>
-      <c r="P151" s="20"/>
-      <c r="Q151" s="20"/>
-      <c r="R151" s="20"/>
-      <c r="S151" s="20"/>
-      <c r="T151" s="20"/>
-      <c r="U151" s="20"/>
-      <c r="V151" s="20"/>
-      <c r="W151" s="20"/>
-      <c r="X151" s="20"/>
-      <c r="Y151" s="20"/>
-      <c r="Z151" s="20"/>
-      <c r="AA151" s="20"/>
-      <c r="AB151" s="20"/>
-      <c r="AC151" s="20"/>
-      <c r="AD151" s="20"/>
-      <c r="AE151" s="20"/>
-      <c r="AF151" s="20"/>
-      <c r="AG151" s="20"/>
+      <c r="B151" s="19"/>
+      <c r="C151" s="19"/>
+      <c r="D151" s="19"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="19"/>
+      <c r="G151" s="19"/>
+      <c r="H151" s="19"/>
+      <c r="I151" s="19"/>
+      <c r="J151" s="19"/>
+      <c r="K151" s="19"/>
+      <c r="L151" s="19"/>
+      <c r="M151" s="19"/>
+      <c r="N151" s="19"/>
+      <c r="O151" s="19"/>
+      <c r="P151" s="19"/>
+      <c r="Q151" s="19"/>
+      <c r="R151" s="19"/>
+      <c r="S151" s="19"/>
+      <c r="T151" s="19"/>
+      <c r="U151" s="19"/>
+      <c r="V151" s="19"/>
+      <c r="W151" s="19"/>
+      <c r="X151" s="19"/>
+      <c r="Y151" s="19"/>
+      <c r="Z151" s="19"/>
+      <c r="AA151" s="19"/>
+      <c r="AB151" s="19"/>
+      <c r="AC151" s="19"/>
+      <c r="AD151" s="19"/>
+      <c r="AE151" s="19"/>
+      <c r="AF151" s="19"/>
+      <c r="AG151" s="19"/>
       <c r="AH151" s="8"/>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4715,11 +4711,11 @@
       <c r="Z153" s="2"/>
       <c r="AH153" s="8"/>
     </row>
-    <row r="154" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="2"/>
       <c r="J154" s="2"/>
-      <c r="R154" s="17"/>
-      <c r="Z154" s="17"/>
+      <c r="R154" s="16"/>
+      <c r="Z154" s="16"/>
       <c r="AH154" s="8"/>
       <c r="AI154" s="1"/>
       <c r="AJ154" s="1"/>
@@ -4785,30 +4781,30 @@
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8"/>
-      <c r="B155" s="17"/>
-      <c r="F155" s="19"/>
-      <c r="H155" s="19"/>
-      <c r="J155" s="17"/>
-      <c r="P155" s="19"/>
-      <c r="R155" s="17"/>
-      <c r="T155" s="19"/>
-      <c r="V155" s="19"/>
-      <c r="X155" s="19"/>
-      <c r="Z155" s="17"/>
+      <c r="B155" s="16"/>
+      <c r="F155" s="18"/>
+      <c r="H155" s="18"/>
+      <c r="J155" s="16"/>
+      <c r="P155" s="18"/>
+      <c r="R155" s="16"/>
+      <c r="T155" s="18"/>
+      <c r="V155" s="18"/>
+      <c r="X155" s="18"/>
+      <c r="Z155" s="16"/>
       <c r="AH155" s="8"/>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="8"/>
-      <c r="V156" s="19"/>
-      <c r="X156" s="19"/>
+      <c r="V156" s="18"/>
+      <c r="X156" s="18"/>
       <c r="AH156" s="8"/>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="8"/>
-      <c r="V157" s="19"/>
-      <c r="X157" s="19"/>
-      <c r="AD157" s="19"/>
-      <c r="AF157" s="19"/>
+      <c r="V157" s="18"/>
+      <c r="X157" s="18"/>
+      <c r="AD157" s="18"/>
+      <c r="AF157" s="18"/>
       <c r="AH157" s="8"/>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4817,38 +4813,38 @@
     </row>
     <row r="159" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="8"/>
-      <c r="B159" s="20"/>
-      <c r="C159" s="20"/>
-      <c r="D159" s="20"/>
-      <c r="E159" s="20"/>
-      <c r="F159" s="20"/>
-      <c r="G159" s="20"/>
-      <c r="H159" s="20"/>
-      <c r="I159" s="20"/>
-      <c r="J159" s="20"/>
-      <c r="K159" s="20"/>
-      <c r="L159" s="20"/>
-      <c r="M159" s="20"/>
-      <c r="N159" s="20"/>
-      <c r="O159" s="20"/>
-      <c r="P159" s="20"/>
-      <c r="Q159" s="20"/>
-      <c r="R159" s="20"/>
-      <c r="S159" s="20"/>
-      <c r="T159" s="20"/>
-      <c r="U159" s="20"/>
-      <c r="V159" s="20"/>
-      <c r="W159" s="20"/>
-      <c r="X159" s="20"/>
-      <c r="Y159" s="20"/>
-      <c r="Z159" s="20"/>
-      <c r="AA159" s="20"/>
-      <c r="AB159" s="20"/>
-      <c r="AC159" s="20"/>
-      <c r="AD159" s="20"/>
-      <c r="AE159" s="20"/>
-      <c r="AF159" s="20"/>
-      <c r="AG159" s="20"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="19"/>
+      <c r="G159" s="19"/>
+      <c r="H159" s="19"/>
+      <c r="I159" s="19"/>
+      <c r="J159" s="19"/>
+      <c r="K159" s="19"/>
+      <c r="L159" s="19"/>
+      <c r="M159" s="19"/>
+      <c r="N159" s="19"/>
+      <c r="O159" s="19"/>
+      <c r="P159" s="19"/>
+      <c r="Q159" s="19"/>
+      <c r="R159" s="19"/>
+      <c r="S159" s="19"/>
+      <c r="T159" s="19"/>
+      <c r="U159" s="19"/>
+      <c r="V159" s="19"/>
+      <c r="W159" s="19"/>
+      <c r="X159" s="19"/>
+      <c r="Y159" s="19"/>
+      <c r="Z159" s="19"/>
+      <c r="AA159" s="19"/>
+      <c r="AB159" s="19"/>
+      <c r="AC159" s="19"/>
+      <c r="AD159" s="19"/>
+      <c r="AE159" s="19"/>
+      <c r="AF159" s="19"/>
+      <c r="AG159" s="19"/>
       <c r="AH159" s="8"/>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4867,11 +4863,11 @@
       <c r="Z161" s="2"/>
       <c r="AH161" s="8"/>
     </row>
-    <row r="162" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="2"/>
       <c r="J162" s="2"/>
-      <c r="R162" s="17"/>
-      <c r="Z162" s="17"/>
+      <c r="R162" s="16"/>
+      <c r="Z162" s="16"/>
       <c r="AH162" s="8"/>
       <c r="AI162" s="1"/>
       <c r="AJ162" s="1"/>
@@ -4937,30 +4933,30 @@
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8"/>
-      <c r="B163" s="17"/>
-      <c r="F163" s="19"/>
-      <c r="H163" s="19"/>
-      <c r="J163" s="17"/>
-      <c r="P163" s="19"/>
-      <c r="R163" s="17"/>
-      <c r="T163" s="19"/>
-      <c r="V163" s="19"/>
-      <c r="X163" s="19"/>
-      <c r="Z163" s="17"/>
+      <c r="B163" s="16"/>
+      <c r="F163" s="18"/>
+      <c r="H163" s="18"/>
+      <c r="J163" s="16"/>
+      <c r="P163" s="18"/>
+      <c r="R163" s="16"/>
+      <c r="T163" s="18"/>
+      <c r="V163" s="18"/>
+      <c r="X163" s="18"/>
+      <c r="Z163" s="16"/>
       <c r="AH163" s="8"/>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="8"/>
-      <c r="V164" s="19"/>
-      <c r="X164" s="19"/>
+      <c r="V164" s="18"/>
+      <c r="X164" s="18"/>
       <c r="AH164" s="8"/>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="8"/>
-      <c r="V165" s="19"/>
-      <c r="X165" s="19"/>
-      <c r="AD165" s="19"/>
-      <c r="AF165" s="19"/>
+      <c r="V165" s="18"/>
+      <c r="X165" s="18"/>
+      <c r="AD165" s="18"/>
+      <c r="AF165" s="18"/>
       <c r="AH165" s="8"/>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4969,38 +4965,38 @@
     </row>
     <row r="167" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="8"/>
-      <c r="B167" s="20"/>
-      <c r="C167" s="20"/>
-      <c r="D167" s="20"/>
-      <c r="E167" s="20"/>
-      <c r="F167" s="20"/>
-      <c r="G167" s="20"/>
-      <c r="H167" s="20"/>
-      <c r="I167" s="20"/>
-      <c r="J167" s="20"/>
-      <c r="K167" s="20"/>
-      <c r="L167" s="20"/>
-      <c r="M167" s="20"/>
-      <c r="N167" s="20"/>
-      <c r="O167" s="20"/>
-      <c r="P167" s="20"/>
-      <c r="Q167" s="20"/>
-      <c r="R167" s="20"/>
-      <c r="S167" s="20"/>
-      <c r="T167" s="20"/>
-      <c r="U167" s="20"/>
-      <c r="V167" s="20"/>
-      <c r="W167" s="20"/>
-      <c r="X167" s="20"/>
-      <c r="Y167" s="20"/>
-      <c r="Z167" s="20"/>
-      <c r="AA167" s="20"/>
-      <c r="AB167" s="20"/>
-      <c r="AC167" s="20"/>
-      <c r="AD167" s="20"/>
-      <c r="AE167" s="20"/>
-      <c r="AF167" s="20"/>
-      <c r="AG167" s="20"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="19"/>
+      <c r="D167" s="19"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="19"/>
+      <c r="G167" s="19"/>
+      <c r="H167" s="19"/>
+      <c r="I167" s="19"/>
+      <c r="J167" s="19"/>
+      <c r="K167" s="19"/>
+      <c r="L167" s="19"/>
+      <c r="M167" s="19"/>
+      <c r="N167" s="19"/>
+      <c r="O167" s="19"/>
+      <c r="P167" s="19"/>
+      <c r="Q167" s="19"/>
+      <c r="R167" s="19"/>
+      <c r="S167" s="19"/>
+      <c r="T167" s="19"/>
+      <c r="U167" s="19"/>
+      <c r="V167" s="19"/>
+      <c r="W167" s="19"/>
+      <c r="X167" s="19"/>
+      <c r="Y167" s="19"/>
+      <c r="Z167" s="19"/>
+      <c r="AA167" s="19"/>
+      <c r="AB167" s="19"/>
+      <c r="AC167" s="19"/>
+      <c r="AD167" s="19"/>
+      <c r="AE167" s="19"/>
+      <c r="AF167" s="19"/>
+      <c r="AG167" s="19"/>
       <c r="AH167" s="8"/>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5019,11 +5015,11 @@
       <c r="Z169" s="2"/>
       <c r="AH169" s="8"/>
     </row>
-    <row r="170" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="2"/>
       <c r="J170" s="2"/>
-      <c r="R170" s="17"/>
-      <c r="Z170" s="17"/>
+      <c r="R170" s="16"/>
+      <c r="Z170" s="16"/>
       <c r="AH170" s="8"/>
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
@@ -5089,30 +5085,30 @@
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="8"/>
-      <c r="B171" s="17"/>
-      <c r="F171" s="19"/>
-      <c r="H171" s="19"/>
-      <c r="J171" s="17"/>
-      <c r="P171" s="19"/>
-      <c r="R171" s="17"/>
-      <c r="T171" s="19"/>
-      <c r="V171" s="19"/>
-      <c r="X171" s="19"/>
-      <c r="Z171" s="17"/>
+      <c r="B171" s="16"/>
+      <c r="F171" s="18"/>
+      <c r="H171" s="18"/>
+      <c r="J171" s="16"/>
+      <c r="P171" s="18"/>
+      <c r="R171" s="16"/>
+      <c r="T171" s="18"/>
+      <c r="V171" s="18"/>
+      <c r="X171" s="18"/>
+      <c r="Z171" s="16"/>
       <c r="AH171" s="8"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="8"/>
-      <c r="V172" s="19"/>
-      <c r="X172" s="19"/>
+      <c r="V172" s="18"/>
+      <c r="X172" s="18"/>
       <c r="AH172" s="8"/>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="8"/>
-      <c r="V173" s="19"/>
-      <c r="X173" s="19"/>
-      <c r="AD173" s="19"/>
-      <c r="AF173" s="19"/>
+      <c r="V173" s="18"/>
+      <c r="X173" s="18"/>
+      <c r="AD173" s="18"/>
+      <c r="AF173" s="18"/>
       <c r="AH173" s="8"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5121,38 +5117,38 @@
     </row>
     <row r="175" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="8"/>
-      <c r="B175" s="20"/>
-      <c r="C175" s="20"/>
-      <c r="D175" s="20"/>
-      <c r="E175" s="20"/>
-      <c r="F175" s="20"/>
-      <c r="G175" s="20"/>
-      <c r="H175" s="20"/>
-      <c r="I175" s="20"/>
-      <c r="J175" s="20"/>
-      <c r="K175" s="20"/>
-      <c r="L175" s="20"/>
-      <c r="M175" s="20"/>
-      <c r="N175" s="20"/>
-      <c r="O175" s="20"/>
-      <c r="P175" s="20"/>
-      <c r="Q175" s="20"/>
-      <c r="R175" s="20"/>
-      <c r="S175" s="20"/>
-      <c r="T175" s="20"/>
-      <c r="U175" s="20"/>
-      <c r="V175" s="20"/>
-      <c r="W175" s="20"/>
-      <c r="X175" s="20"/>
-      <c r="Y175" s="20"/>
-      <c r="Z175" s="20"/>
-      <c r="AA175" s="20"/>
-      <c r="AB175" s="20"/>
-      <c r="AC175" s="20"/>
-      <c r="AD175" s="20"/>
-      <c r="AE175" s="20"/>
-      <c r="AF175" s="20"/>
-      <c r="AG175" s="20"/>
+      <c r="B175" s="19"/>
+      <c r="C175" s="19"/>
+      <c r="D175" s="19"/>
+      <c r="E175" s="19"/>
+      <c r="F175" s="19"/>
+      <c r="G175" s="19"/>
+      <c r="H175" s="19"/>
+      <c r="I175" s="19"/>
+      <c r="J175" s="19"/>
+      <c r="K175" s="19"/>
+      <c r="L175" s="19"/>
+      <c r="M175" s="19"/>
+      <c r="N175" s="19"/>
+      <c r="O175" s="19"/>
+      <c r="P175" s="19"/>
+      <c r="Q175" s="19"/>
+      <c r="R175" s="19"/>
+      <c r="S175" s="19"/>
+      <c r="T175" s="19"/>
+      <c r="U175" s="19"/>
+      <c r="V175" s="19"/>
+      <c r="W175" s="19"/>
+      <c r="X175" s="19"/>
+      <c r="Y175" s="19"/>
+      <c r="Z175" s="19"/>
+      <c r="AA175" s="19"/>
+      <c r="AB175" s="19"/>
+      <c r="AC175" s="19"/>
+      <c r="AD175" s="19"/>
+      <c r="AE175" s="19"/>
+      <c r="AF175" s="19"/>
+      <c r="AG175" s="19"/>
       <c r="AH175" s="8"/>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5171,11 +5167,11 @@
       <c r="Z177" s="2"/>
       <c r="AH177" s="8"/>
     </row>
-    <row r="178" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="2"/>
       <c r="J178" s="2"/>
-      <c r="R178" s="17"/>
-      <c r="Z178" s="17"/>
+      <c r="R178" s="16"/>
+      <c r="Z178" s="16"/>
       <c r="AH178" s="8"/>
       <c r="AI178" s="1"/>
       <c r="AJ178" s="1"/>
@@ -5241,30 +5237,30 @@
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="8"/>
-      <c r="B179" s="17"/>
-      <c r="F179" s="19"/>
-      <c r="H179" s="19"/>
-      <c r="J179" s="17"/>
-      <c r="P179" s="19"/>
-      <c r="R179" s="17"/>
-      <c r="T179" s="19"/>
-      <c r="V179" s="19"/>
-      <c r="X179" s="19"/>
-      <c r="Z179" s="17"/>
+      <c r="B179" s="16"/>
+      <c r="F179" s="18"/>
+      <c r="H179" s="18"/>
+      <c r="J179" s="16"/>
+      <c r="P179" s="18"/>
+      <c r="R179" s="16"/>
+      <c r="T179" s="18"/>
+      <c r="V179" s="18"/>
+      <c r="X179" s="18"/>
+      <c r="Z179" s="16"/>
       <c r="AH179" s="8"/>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="8"/>
-      <c r="V180" s="19"/>
-      <c r="X180" s="19"/>
+      <c r="V180" s="18"/>
+      <c r="X180" s="18"/>
       <c r="AH180" s="8"/>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="8"/>
-      <c r="V181" s="19"/>
-      <c r="X181" s="19"/>
-      <c r="AD181" s="19"/>
-      <c r="AF181" s="19"/>
+      <c r="V181" s="18"/>
+      <c r="X181" s="18"/>
+      <c r="AD181" s="18"/>
+      <c r="AF181" s="18"/>
       <c r="AH181" s="8"/>
     </row>
     <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5273,38 +5269,38 @@
     </row>
     <row r="183" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="8"/>
-      <c r="B183" s="20"/>
-      <c r="C183" s="20"/>
-      <c r="D183" s="20"/>
-      <c r="E183" s="20"/>
-      <c r="F183" s="20"/>
-      <c r="G183" s="20"/>
-      <c r="H183" s="20"/>
-      <c r="I183" s="20"/>
-      <c r="J183" s="20"/>
-      <c r="K183" s="20"/>
-      <c r="L183" s="20"/>
-      <c r="M183" s="20"/>
-      <c r="N183" s="20"/>
-      <c r="O183" s="20"/>
-      <c r="P183" s="20"/>
-      <c r="Q183" s="20"/>
-      <c r="R183" s="20"/>
-      <c r="S183" s="20"/>
-      <c r="T183" s="20"/>
-      <c r="U183" s="20"/>
-      <c r="V183" s="20"/>
-      <c r="W183" s="20"/>
-      <c r="X183" s="20"/>
-      <c r="Y183" s="20"/>
-      <c r="Z183" s="20"/>
-      <c r="AA183" s="20"/>
-      <c r="AB183" s="20"/>
-      <c r="AC183" s="20"/>
-      <c r="AD183" s="20"/>
-      <c r="AE183" s="20"/>
-      <c r="AF183" s="20"/>
-      <c r="AG183" s="20"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="19"/>
+      <c r="D183" s="19"/>
+      <c r="E183" s="19"/>
+      <c r="F183" s="19"/>
+      <c r="G183" s="19"/>
+      <c r="H183" s="19"/>
+      <c r="I183" s="19"/>
+      <c r="J183" s="19"/>
+      <c r="K183" s="19"/>
+      <c r="L183" s="19"/>
+      <c r="M183" s="19"/>
+      <c r="N183" s="19"/>
+      <c r="O183" s="19"/>
+      <c r="P183" s="19"/>
+      <c r="Q183" s="19"/>
+      <c r="R183" s="19"/>
+      <c r="S183" s="19"/>
+      <c r="T183" s="19"/>
+      <c r="U183" s="19"/>
+      <c r="V183" s="19"/>
+      <c r="W183" s="19"/>
+      <c r="X183" s="19"/>
+      <c r="Y183" s="19"/>
+      <c r="Z183" s="19"/>
+      <c r="AA183" s="19"/>
+      <c r="AB183" s="19"/>
+      <c r="AC183" s="19"/>
+      <c r="AD183" s="19"/>
+      <c r="AE183" s="19"/>
+      <c r="AF183" s="19"/>
+      <c r="AG183" s="19"/>
       <c r="AH183" s="8"/>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5323,11 +5319,11 @@
       <c r="Z185" s="2"/>
       <c r="AH185" s="8"/>
     </row>
-    <row r="186" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="2"/>
       <c r="J186" s="2"/>
-      <c r="R186" s="17"/>
-      <c r="Z186" s="17"/>
+      <c r="R186" s="16"/>
+      <c r="Z186" s="16"/>
       <c r="AH186" s="8"/>
       <c r="AI186" s="1"/>
       <c r="AJ186" s="1"/>
@@ -5393,30 +5389,30 @@
     </row>
     <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="8"/>
-      <c r="B187" s="17"/>
-      <c r="F187" s="19"/>
-      <c r="H187" s="19"/>
-      <c r="J187" s="17"/>
-      <c r="P187" s="19"/>
-      <c r="R187" s="17"/>
-      <c r="T187" s="19"/>
-      <c r="V187" s="19"/>
-      <c r="X187" s="19"/>
-      <c r="Z187" s="17"/>
+      <c r="B187" s="16"/>
+      <c r="F187" s="18"/>
+      <c r="H187" s="18"/>
+      <c r="J187" s="16"/>
+      <c r="P187" s="18"/>
+      <c r="R187" s="16"/>
+      <c r="T187" s="18"/>
+      <c r="V187" s="18"/>
+      <c r="X187" s="18"/>
+      <c r="Z187" s="16"/>
       <c r="AH187" s="8"/>
     </row>
     <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="8"/>
-      <c r="V188" s="19"/>
-      <c r="X188" s="19"/>
+      <c r="V188" s="18"/>
+      <c r="X188" s="18"/>
       <c r="AH188" s="8"/>
     </row>
     <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="8"/>
-      <c r="V189" s="19"/>
-      <c r="X189" s="19"/>
-      <c r="AD189" s="19"/>
-      <c r="AF189" s="19"/>
+      <c r="V189" s="18"/>
+      <c r="X189" s="18"/>
+      <c r="AD189" s="18"/>
+      <c r="AF189" s="18"/>
       <c r="AH189" s="8"/>
     </row>
     <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5425,38 +5421,38 @@
     </row>
     <row r="191" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="8"/>
-      <c r="B191" s="20"/>
-      <c r="C191" s="20"/>
-      <c r="D191" s="20"/>
-      <c r="E191" s="20"/>
-      <c r="F191" s="20"/>
-      <c r="G191" s="20"/>
-      <c r="H191" s="20"/>
-      <c r="I191" s="20"/>
-      <c r="J191" s="20"/>
-      <c r="K191" s="20"/>
-      <c r="L191" s="20"/>
-      <c r="M191" s="20"/>
-      <c r="N191" s="20"/>
-      <c r="O191" s="20"/>
-      <c r="P191" s="20"/>
-      <c r="Q191" s="20"/>
-      <c r="R191" s="20"/>
-      <c r="S191" s="20"/>
-      <c r="T191" s="20"/>
-      <c r="U191" s="20"/>
-      <c r="V191" s="20"/>
-      <c r="W191" s="20"/>
-      <c r="X191" s="20"/>
-      <c r="Y191" s="20"/>
-      <c r="Z191" s="20"/>
-      <c r="AA191" s="20"/>
-      <c r="AB191" s="20"/>
-      <c r="AC191" s="20"/>
-      <c r="AD191" s="20"/>
-      <c r="AE191" s="20"/>
-      <c r="AF191" s="20"/>
-      <c r="AG191" s="20"/>
+      <c r="B191" s="19"/>
+      <c r="C191" s="19"/>
+      <c r="D191" s="19"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="19"/>
+      <c r="G191" s="19"/>
+      <c r="H191" s="19"/>
+      <c r="I191" s="19"/>
+      <c r="J191" s="19"/>
+      <c r="K191" s="19"/>
+      <c r="L191" s="19"/>
+      <c r="M191" s="19"/>
+      <c r="N191" s="19"/>
+      <c r="O191" s="19"/>
+      <c r="P191" s="19"/>
+      <c r="Q191" s="19"/>
+      <c r="R191" s="19"/>
+      <c r="S191" s="19"/>
+      <c r="T191" s="19"/>
+      <c r="U191" s="19"/>
+      <c r="V191" s="19"/>
+      <c r="W191" s="19"/>
+      <c r="X191" s="19"/>
+      <c r="Y191" s="19"/>
+      <c r="Z191" s="19"/>
+      <c r="AA191" s="19"/>
+      <c r="AB191" s="19"/>
+      <c r="AC191" s="19"/>
+      <c r="AD191" s="19"/>
+      <c r="AE191" s="19"/>
+      <c r="AF191" s="19"/>
+      <c r="AG191" s="19"/>
       <c r="AH191" s="8"/>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5475,11 +5471,11 @@
       <c r="Z193" s="2"/>
       <c r="AH193" s="8"/>
     </row>
-    <row r="194" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="2"/>
       <c r="J194" s="2"/>
-      <c r="R194" s="17"/>
-      <c r="Z194" s="17"/>
+      <c r="R194" s="16"/>
+      <c r="Z194" s="16"/>
       <c r="AH194" s="8"/>
       <c r="AI194" s="1"/>
       <c r="AJ194" s="1"/>
@@ -5545,30 +5541,30 @@
     </row>
     <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="8"/>
-      <c r="B195" s="17"/>
-      <c r="F195" s="19"/>
-      <c r="H195" s="19"/>
-      <c r="J195" s="17"/>
-      <c r="P195" s="19"/>
-      <c r="R195" s="17"/>
-      <c r="T195" s="19"/>
-      <c r="V195" s="19"/>
-      <c r="X195" s="19"/>
-      <c r="Z195" s="17"/>
+      <c r="B195" s="16"/>
+      <c r="F195" s="18"/>
+      <c r="H195" s="18"/>
+      <c r="J195" s="16"/>
+      <c r="P195" s="18"/>
+      <c r="R195" s="16"/>
+      <c r="T195" s="18"/>
+      <c r="V195" s="18"/>
+      <c r="X195" s="18"/>
+      <c r="Z195" s="16"/>
       <c r="AH195" s="8"/>
     </row>
     <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="8"/>
-      <c r="V196" s="19"/>
-      <c r="X196" s="19"/>
+      <c r="V196" s="18"/>
+      <c r="X196" s="18"/>
       <c r="AH196" s="8"/>
     </row>
     <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="8"/>
-      <c r="V197" s="19"/>
-      <c r="X197" s="19"/>
-      <c r="AD197" s="19"/>
-      <c r="AF197" s="19"/>
+      <c r="V197" s="18"/>
+      <c r="X197" s="18"/>
+      <c r="AD197" s="18"/>
+      <c r="AF197" s="18"/>
       <c r="AH197" s="8"/>
     </row>
     <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5577,38 +5573,38 @@
     </row>
     <row r="199" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="8"/>
-      <c r="B199" s="20"/>
-      <c r="C199" s="20"/>
-      <c r="D199" s="20"/>
-      <c r="E199" s="20"/>
-      <c r="F199" s="20"/>
-      <c r="G199" s="20"/>
-      <c r="H199" s="20"/>
-      <c r="I199" s="20"/>
-      <c r="J199" s="20"/>
-      <c r="K199" s="20"/>
-      <c r="L199" s="20"/>
-      <c r="M199" s="20"/>
-      <c r="N199" s="20"/>
-      <c r="O199" s="20"/>
-      <c r="P199" s="20"/>
-      <c r="Q199" s="20"/>
-      <c r="R199" s="20"/>
-      <c r="S199" s="20"/>
-      <c r="T199" s="20"/>
-      <c r="U199" s="20"/>
-      <c r="V199" s="20"/>
-      <c r="W199" s="20"/>
-      <c r="X199" s="20"/>
-      <c r="Y199" s="20"/>
-      <c r="Z199" s="20"/>
-      <c r="AA199" s="20"/>
-      <c r="AB199" s="20"/>
-      <c r="AC199" s="20"/>
-      <c r="AD199" s="20"/>
-      <c r="AE199" s="20"/>
-      <c r="AF199" s="20"/>
-      <c r="AG199" s="20"/>
+      <c r="B199" s="19"/>
+      <c r="C199" s="19"/>
+      <c r="D199" s="19"/>
+      <c r="E199" s="19"/>
+      <c r="F199" s="19"/>
+      <c r="G199" s="19"/>
+      <c r="H199" s="19"/>
+      <c r="I199" s="19"/>
+      <c r="J199" s="19"/>
+      <c r="K199" s="19"/>
+      <c r="L199" s="19"/>
+      <c r="M199" s="19"/>
+      <c r="N199" s="19"/>
+      <c r="O199" s="19"/>
+      <c r="P199" s="19"/>
+      <c r="Q199" s="19"/>
+      <c r="R199" s="19"/>
+      <c r="S199" s="19"/>
+      <c r="T199" s="19"/>
+      <c r="U199" s="19"/>
+      <c r="V199" s="19"/>
+      <c r="W199" s="19"/>
+      <c r="X199" s="19"/>
+      <c r="Y199" s="19"/>
+      <c r="Z199" s="19"/>
+      <c r="AA199" s="19"/>
+      <c r="AB199" s="19"/>
+      <c r="AC199" s="19"/>
+      <c r="AD199" s="19"/>
+      <c r="AE199" s="19"/>
+      <c r="AF199" s="19"/>
+      <c r="AG199" s="19"/>
       <c r="AH199" s="8"/>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5627,11 +5623,11 @@
       <c r="Z201" s="2"/>
       <c r="AH201" s="8"/>
     </row>
-    <row r="202" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="2"/>
       <c r="J202" s="2"/>
-      <c r="R202" s="17"/>
-      <c r="Z202" s="17"/>
+      <c r="R202" s="16"/>
+      <c r="Z202" s="16"/>
       <c r="AH202" s="8"/>
       <c r="AI202" s="1"/>
       <c r="AJ202" s="1"/>
@@ -5697,30 +5693,30 @@
     </row>
     <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="8"/>
-      <c r="B203" s="17"/>
-      <c r="F203" s="19"/>
-      <c r="H203" s="19"/>
-      <c r="J203" s="17"/>
-      <c r="P203" s="19"/>
-      <c r="R203" s="17"/>
-      <c r="T203" s="19"/>
-      <c r="V203" s="19"/>
-      <c r="X203" s="19"/>
-      <c r="Z203" s="17"/>
+      <c r="B203" s="16"/>
+      <c r="F203" s="18"/>
+      <c r="H203" s="18"/>
+      <c r="J203" s="16"/>
+      <c r="P203" s="18"/>
+      <c r="R203" s="16"/>
+      <c r="T203" s="18"/>
+      <c r="V203" s="18"/>
+      <c r="X203" s="18"/>
+      <c r="Z203" s="16"/>
       <c r="AH203" s="8"/>
     </row>
     <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="8"/>
-      <c r="V204" s="19"/>
-      <c r="X204" s="19"/>
+      <c r="V204" s="18"/>
+      <c r="X204" s="18"/>
       <c r="AH204" s="8"/>
     </row>
     <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="8"/>
-      <c r="V205" s="19"/>
-      <c r="X205" s="19"/>
-      <c r="AD205" s="19"/>
-      <c r="AF205" s="19"/>
+      <c r="V205" s="18"/>
+      <c r="X205" s="18"/>
+      <c r="AD205" s="18"/>
+      <c r="AF205" s="18"/>
       <c r="AH205" s="8"/>
     </row>
     <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5729,38 +5725,38 @@
     </row>
     <row r="207" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="8"/>
-      <c r="B207" s="20"/>
-      <c r="C207" s="20"/>
-      <c r="D207" s="20"/>
-      <c r="E207" s="20"/>
-      <c r="F207" s="20"/>
-      <c r="G207" s="20"/>
-      <c r="H207" s="20"/>
-      <c r="I207" s="20"/>
-      <c r="J207" s="20"/>
-      <c r="K207" s="20"/>
-      <c r="L207" s="20"/>
-      <c r="M207" s="20"/>
-      <c r="N207" s="20"/>
-      <c r="O207" s="20"/>
-      <c r="P207" s="20"/>
-      <c r="Q207" s="20"/>
-      <c r="R207" s="20"/>
-      <c r="S207" s="20"/>
-      <c r="T207" s="20"/>
-      <c r="U207" s="20"/>
-      <c r="V207" s="20"/>
-      <c r="W207" s="20"/>
-      <c r="X207" s="20"/>
-      <c r="Y207" s="20"/>
-      <c r="Z207" s="20"/>
-      <c r="AA207" s="20"/>
-      <c r="AB207" s="20"/>
-      <c r="AC207" s="20"/>
-      <c r="AD207" s="20"/>
-      <c r="AE207" s="20"/>
-      <c r="AF207" s="20"/>
-      <c r="AG207" s="20"/>
+      <c r="B207" s="19"/>
+      <c r="C207" s="19"/>
+      <c r="D207" s="19"/>
+      <c r="E207" s="19"/>
+      <c r="F207" s="19"/>
+      <c r="G207" s="19"/>
+      <c r="H207" s="19"/>
+      <c r="I207" s="19"/>
+      <c r="J207" s="19"/>
+      <c r="K207" s="19"/>
+      <c r="L207" s="19"/>
+      <c r="M207" s="19"/>
+      <c r="N207" s="19"/>
+      <c r="O207" s="19"/>
+      <c r="P207" s="19"/>
+      <c r="Q207" s="19"/>
+      <c r="R207" s="19"/>
+      <c r="S207" s="19"/>
+      <c r="T207" s="19"/>
+      <c r="U207" s="19"/>
+      <c r="V207" s="19"/>
+      <c r="W207" s="19"/>
+      <c r="X207" s="19"/>
+      <c r="Y207" s="19"/>
+      <c r="Z207" s="19"/>
+      <c r="AA207" s="19"/>
+      <c r="AB207" s="19"/>
+      <c r="AC207" s="19"/>
+      <c r="AD207" s="19"/>
+      <c r="AE207" s="19"/>
+      <c r="AF207" s="19"/>
+      <c r="AG207" s="19"/>
       <c r="AH207" s="8"/>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,11 +5775,11 @@
       <c r="Z209" s="2"/>
       <c r="AH209" s="8"/>
     </row>
-    <row r="210" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="2"/>
       <c r="J210" s="2"/>
-      <c r="R210" s="17"/>
-      <c r="Z210" s="17"/>
+      <c r="R210" s="16"/>
+      <c r="Z210" s="16"/>
       <c r="AH210" s="8"/>
       <c r="AI210" s="1"/>
       <c r="AJ210" s="1"/>
@@ -5849,30 +5845,30 @@
     </row>
     <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="8"/>
-      <c r="B211" s="17"/>
-      <c r="F211" s="19"/>
-      <c r="H211" s="19"/>
-      <c r="J211" s="17"/>
-      <c r="P211" s="19"/>
-      <c r="R211" s="17"/>
-      <c r="T211" s="19"/>
-      <c r="V211" s="19"/>
-      <c r="X211" s="19"/>
-      <c r="Z211" s="17"/>
+      <c r="B211" s="16"/>
+      <c r="F211" s="18"/>
+      <c r="H211" s="18"/>
+      <c r="J211" s="16"/>
+      <c r="P211" s="18"/>
+      <c r="R211" s="16"/>
+      <c r="T211" s="18"/>
+      <c r="V211" s="18"/>
+      <c r="X211" s="18"/>
+      <c r="Z211" s="16"/>
       <c r="AH211" s="8"/>
     </row>
     <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="8"/>
-      <c r="V212" s="19"/>
-      <c r="X212" s="19"/>
+      <c r="V212" s="18"/>
+      <c r="X212" s="18"/>
       <c r="AH212" s="8"/>
     </row>
     <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="8"/>
-      <c r="V213" s="19"/>
-      <c r="X213" s="19"/>
-      <c r="AD213" s="19"/>
-      <c r="AF213" s="19"/>
+      <c r="V213" s="18"/>
+      <c r="X213" s="18"/>
+      <c r="AD213" s="18"/>
+      <c r="AF213" s="18"/>
       <c r="AH213" s="8"/>
     </row>
     <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5881,38 +5877,38 @@
     </row>
     <row r="215" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="8"/>
-      <c r="B215" s="20"/>
-      <c r="C215" s="20"/>
-      <c r="D215" s="20"/>
-      <c r="E215" s="20"/>
-      <c r="F215" s="20"/>
-      <c r="G215" s="20"/>
-      <c r="H215" s="20"/>
-      <c r="I215" s="20"/>
-      <c r="J215" s="20"/>
-      <c r="K215" s="20"/>
-      <c r="L215" s="20"/>
-      <c r="M215" s="20"/>
-      <c r="N215" s="20"/>
-      <c r="O215" s="20"/>
-      <c r="P215" s="20"/>
-      <c r="Q215" s="20"/>
-      <c r="R215" s="20"/>
-      <c r="S215" s="20"/>
-      <c r="T215" s="20"/>
-      <c r="U215" s="20"/>
-      <c r="V215" s="20"/>
-      <c r="W215" s="20"/>
-      <c r="X215" s="20"/>
-      <c r="Y215" s="20"/>
-      <c r="Z215" s="20"/>
-      <c r="AA215" s="20"/>
-      <c r="AB215" s="20"/>
-      <c r="AC215" s="20"/>
-      <c r="AD215" s="20"/>
-      <c r="AE215" s="20"/>
-      <c r="AF215" s="20"/>
-      <c r="AG215" s="20"/>
+      <c r="B215" s="19"/>
+      <c r="C215" s="19"/>
+      <c r="D215" s="19"/>
+      <c r="E215" s="19"/>
+      <c r="F215" s="19"/>
+      <c r="G215" s="19"/>
+      <c r="H215" s="19"/>
+      <c r="I215" s="19"/>
+      <c r="J215" s="19"/>
+      <c r="K215" s="19"/>
+      <c r="L215" s="19"/>
+      <c r="M215" s="19"/>
+      <c r="N215" s="19"/>
+      <c r="O215" s="19"/>
+      <c r="P215" s="19"/>
+      <c r="Q215" s="19"/>
+      <c r="R215" s="19"/>
+      <c r="S215" s="19"/>
+      <c r="T215" s="19"/>
+      <c r="U215" s="19"/>
+      <c r="V215" s="19"/>
+      <c r="W215" s="19"/>
+      <c r="X215" s="19"/>
+      <c r="Y215" s="19"/>
+      <c r="Z215" s="19"/>
+      <c r="AA215" s="19"/>
+      <c r="AB215" s="19"/>
+      <c r="AC215" s="19"/>
+      <c r="AD215" s="19"/>
+      <c r="AE215" s="19"/>
+      <c r="AF215" s="19"/>
+      <c r="AG215" s="19"/>
       <c r="AH215" s="8"/>
     </row>
     <row r="216" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,11 +5927,11 @@
       <c r="Z217" s="2"/>
       <c r="AH217" s="8"/>
     </row>
-    <row r="218" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="2"/>
       <c r="J218" s="2"/>
-      <c r="R218" s="17"/>
-      <c r="Z218" s="17"/>
+      <c r="R218" s="16"/>
+      <c r="Z218" s="16"/>
       <c r="AH218" s="8"/>
       <c r="AI218" s="1"/>
       <c r="AJ218" s="1"/>
@@ -6000,6 +5996,22 @@
       <c r="CQ218" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="B8:Q8"/>
+    <mergeCell ref="B9:AG9"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="B14:Q14"/>
+    <mergeCell ref="B15:Q15"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>